<commit_message>
Separated Plag and Kspar into 2 sheets
</commit_message>
<xml_diff>
--- a/Examples/Amphibole/Amphibole_Liquids.xlsx
+++ b/Examples/Amphibole/Amphibole_Liquids.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\penny\OneDrive - Oregon State University\Postdoc\PyMME\MyBarometers\Thermobar_outer\Examples\Amphibole\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B60C74B-D60F-49A1-80B3-5A8E650C0DA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{669BEEE2-9FE4-46B7-BF36-82F7E0C46D6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17790" xr2:uid="{5C7BD346-92C0-4F53-93F6-E0A947C2FF67}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{5C7BD346-92C0-4F53-93F6-E0A947C2FF67}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -598,7 +598,7 @@
   <dimension ref="A1:X23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+      <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>